<commit_message>
week 09 finished coding
</commit_message>
<xml_diff>
--- a/timesheets/timeshseet.xlsx
+++ b/timesheets/timeshseet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AB-Tech\semester 5\web289\timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EF419E-5636-4E6F-9BA3-831C74D3D86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27003978-8D25-4FFA-BADF-412D485C7A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="560" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="560" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="44">
   <si>
     <t>Weekley Total</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -151,6 +151,45 @@
   </si>
   <si>
     <t>finishing sql</t>
+  </si>
+  <si>
+    <t>finished sql</t>
+  </si>
+  <si>
+    <t>making sure everyting is finished</t>
+  </si>
+  <si>
+    <t>finalising</t>
+  </si>
+  <si>
+    <t>in class fixing mistakes</t>
+  </si>
+  <si>
+    <t>file structure and blank files for website</t>
+  </si>
+  <si>
+    <t>finalising file structure started coding</t>
+  </si>
+  <si>
+    <t>coding website</t>
+  </si>
+  <si>
+    <t>working on website backend/classes</t>
+  </si>
+  <si>
+    <t>working on website backend/functions</t>
+  </si>
+  <si>
+    <t>working on website frontend</t>
+  </si>
+  <si>
+    <t>class time</t>
+  </si>
+  <si>
+    <t>working on session class/ login</t>
+  </si>
+  <si>
+    <t>working on session class/ restricting content based on user</t>
   </si>
 </sst>
 </file>
@@ -254,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -277,7 +316,6 @@
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,7 +656,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A3" sqref="A3:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -647,7 +685,7 @@
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>43473</v>
+        <v>43838</v>
       </c>
       <c r="B2" s="6">
         <v>0.52083333333333337</v>
@@ -665,7 +703,7 @@
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>43473</v>
+        <v>43838</v>
       </c>
       <c r="B3" s="6">
         <v>0.70833333333333337</v>
@@ -683,7 +721,7 @@
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>43474</v>
+        <v>43839</v>
       </c>
       <c r="B4" s="8">
         <v>0.70833333333333337</v>
@@ -701,7 +739,7 @@
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>43475</v>
+        <v>43840</v>
       </c>
       <c r="B5" s="6">
         <v>0.41666666666666669</v>
@@ -719,7 +757,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
-        <v>43476</v>
+        <v>43841</v>
       </c>
       <c r="B6" s="6">
         <v>0.5</v>
@@ -856,7 +894,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 9'!E21</f>
-        <v>1.7986111111111103</v>
+        <v>2.1111111111111103</v>
       </c>
     </row>
   </sheetData>
@@ -921,7 +959,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 10'!E21</f>
-        <v>1.7986111111111103</v>
+        <v>2.1111111111111103</v>
       </c>
     </row>
   </sheetData>
@@ -986,7 +1024,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 11'!E21</f>
-        <v>1.7986111111111103</v>
+        <v>2.1111111111111103</v>
       </c>
     </row>
   </sheetData>
@@ -1051,7 +1089,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 12'!E21</f>
-        <v>1.7986111111111103</v>
+        <v>2.1111111111111103</v>
       </c>
     </row>
   </sheetData>
@@ -1116,7 +1154,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 13'!E21</f>
-        <v>1.7986111111111103</v>
+        <v>2.1111111111111103</v>
       </c>
     </row>
   </sheetData>
@@ -1181,7 +1219,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>1.7986111111111103</v>
+        <v>2.1111111111111103</v>
       </c>
     </row>
   </sheetData>
@@ -1246,7 +1284,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 14'!E21</f>
-        <v>1.7986111111111103</v>
+        <v>2.1111111111111103</v>
       </c>
     </row>
   </sheetData>
@@ -1266,7 +1304,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1294,7 +1332,7 @@
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>43477</v>
+        <v>43842</v>
       </c>
       <c r="B2" s="9">
         <v>0.89583333333333337</v>
@@ -1312,7 +1350,7 @@
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>43478</v>
+        <v>43843</v>
       </c>
       <c r="B3" s="9">
         <v>0.89583333333333337</v>
@@ -1330,7 +1368,7 @@
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>43479</v>
+        <v>43844</v>
       </c>
       <c r="B4" s="10">
         <v>0.58333333333333337</v>
@@ -1348,7 +1386,7 @@
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>43480</v>
+        <v>43845</v>
       </c>
       <c r="B5" s="10">
         <v>0.52083333333333337</v>
@@ -1366,7 +1404,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
-        <v>43481</v>
+        <v>43846</v>
       </c>
       <c r="B6" s="9">
         <v>0.58333333333333337</v>
@@ -1384,7 +1422,7 @@
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
-        <v>43482</v>
+        <v>43847</v>
       </c>
       <c r="B7" s="10">
         <v>0.66666666666666663</v>
@@ -1402,7 +1440,7 @@
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
-        <v>43483</v>
+        <v>43848</v>
       </c>
       <c r="B8" s="10">
         <v>0.5</v>
@@ -1457,7 +1495,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1485,7 +1523,7 @@
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>43484</v>
+        <v>43849</v>
       </c>
       <c r="B2" s="10">
         <v>0.89583333333333337</v>
@@ -1503,7 +1541,7 @@
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>43485</v>
+        <v>43850</v>
       </c>
       <c r="B3" s="10">
         <v>0.89583333333333337</v>
@@ -1521,7 +1559,7 @@
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>43486</v>
+        <v>43851</v>
       </c>
       <c r="B4" s="10">
         <v>0.58333333333333337</v>
@@ -1539,7 +1577,7 @@
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>43487</v>
+        <v>43852</v>
       </c>
       <c r="B5" s="10">
         <v>0.6875</v>
@@ -1557,7 +1595,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
-        <v>43488</v>
+        <v>43853</v>
       </c>
       <c r="B6" s="10">
         <v>0.70833333333333337</v>
@@ -1575,7 +1613,7 @@
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
-        <v>43489</v>
+        <v>43854</v>
       </c>
       <c r="B7" s="10">
         <v>0.54166666666666663</v>
@@ -1593,7 +1631,7 @@
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
-        <v>43490</v>
+        <v>43855</v>
       </c>
       <c r="B8" s="10">
         <v>0.58333333333333337</v>
@@ -1657,7 +1695,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A2" sqref="A2:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1686,7 +1724,7 @@
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>43491</v>
+        <v>43856</v>
       </c>
       <c r="B2" s="10">
         <v>0.89583333333333337</v>
@@ -1704,7 +1742,7 @@
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>43492</v>
+        <v>43857</v>
       </c>
       <c r="B3" s="10">
         <v>0.89583333333333337</v>
@@ -1722,7 +1760,7 @@
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>43493</v>
+        <v>43858</v>
       </c>
       <c r="B4" s="9">
         <v>0.58333333333333337</v>
@@ -1740,7 +1778,7 @@
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>43494</v>
+        <v>43859</v>
       </c>
       <c r="B5" s="10">
         <v>0.52083333333333337</v>
@@ -1758,7 +1796,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
-        <v>43495</v>
+        <v>43860</v>
       </c>
       <c r="B6" s="9">
         <v>0.70833333333333337</v>
@@ -1776,7 +1814,7 @@
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
-        <v>43496</v>
+        <v>43861</v>
       </c>
       <c r="B7" s="10">
         <v>0.58333333333333337</v>
@@ -1794,7 +1832,7 @@
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
-        <v>43497</v>
+        <v>43862</v>
       </c>
       <c r="B8" s="10">
         <v>0.58333333333333337</v>
@@ -1881,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1910,7 +1948,7 @@
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
-        <v>43498</v>
+        <v>43863</v>
       </c>
       <c r="B2" s="10">
         <v>0.89583333333333337</v>
@@ -1928,7 +1966,7 @@
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
-        <v>43499</v>
+        <v>43864</v>
       </c>
       <c r="B3" s="10">
         <v>0.89583333333333337</v>
@@ -1946,7 +1984,7 @@
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
-        <v>43500</v>
+        <v>43865</v>
       </c>
       <c r="B4" s="10">
         <v>0.58333333333333337</v>
@@ -1964,7 +2002,7 @@
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>43501</v>
+        <v>43866</v>
       </c>
       <c r="B5" s="10">
         <v>0.52083333333333337</v>
@@ -1972,7 +2010,7 @@
       <c r="C5" s="10">
         <v>0.59375</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="E5" s="6">
@@ -1982,7 +2020,7 @@
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
-        <v>43502</v>
+        <v>43867</v>
       </c>
       <c r="B6" s="10">
         <v>0.64583333333333337</v>
@@ -1990,7 +2028,7 @@
       <c r="C6" s="10">
         <v>0.70833333333333337</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="7" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="6">
@@ -2000,20 +2038,20 @@
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
-        <v>43503</v>
+        <v>43868</v>
       </c>
       <c r="B7" s="6">
-        <v>4.1666666666666664E-2</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="C7" s="10">
         <v>0.58333333333333337</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="7" t="s">
         <v>27</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" si="0"/>
-        <v>0.54166666666666674</v>
+        <v>4.1666666666666741E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2025,7 +2063,7 @@
       </c>
       <c r="E20" s="13">
         <f>SUM(E2:E19)</f>
-        <v>0.76041666666666652</v>
+        <v>0.26041666666666652</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2034,7 +2072,7 @@
       </c>
       <c r="E21" s="13">
         <f>E20+'Week 4'!E21</f>
-        <v>1.7986111111111103</v>
+        <v>1.2986111111111103</v>
       </c>
     </row>
   </sheetData>
@@ -2058,7 +2096,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2084,22 +2122,158 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>43869</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="6">
+        <f>C2-B2</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>43870</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E9" si="0">C3-B3</f>
+        <v>2.0833333333333259E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>43871</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>43872</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666664E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>43873</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>43874</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>43875</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0.6875</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>43876</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="6">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>0.29166666666666652</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="13">
         <f>E20+'Week 5'!E21</f>
-        <v>1.7986111111111103</v>
+        <v>1.5902777777777768</v>
       </c>
     </row>
   </sheetData>
@@ -2107,7 +2281,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Verdana,Bold"&amp;14Internet Technologies Project Time Sheet</oddHeader>
+    <oddHeader>&amp;C&amp;"Verdana,Bold"&amp;14Internet Technologies Project Time Sheet&amp;RBen Harwood</oddHeader>
     <oddFooter>&amp;C&amp;A</oddFooter>
   </headerFooter>
   <extLst>
@@ -2123,7 +2297,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2149,22 +2323,148 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>43877</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.875</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="6">
+        <f>C2-B2</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>43878</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0.875</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" ref="E3:E8" si="0">C3-B3</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>43879</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>43880</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>43881</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>43882</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>4.1666666666666741E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>43883</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0.625</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="13">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>0.27083333333333359</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="13">
         <f>E20+'Week 6'!E21</f>
-        <v>1.7986111111111103</v>
+        <v>1.8611111111111103</v>
       </c>
     </row>
   </sheetData>
@@ -2172,7 +2472,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Verdana,Bold"&amp;14Internet Technologies Project Time Sheet</oddHeader>
+    <oddHeader>&amp;C&amp;"Verdana,Bold"&amp;14Internet Technologies Project Time Sheet&amp;RBen Harwood</oddHeader>
     <oddFooter>&amp;C&amp;A</oddFooter>
   </headerFooter>
   <extLst>
@@ -2187,8 +2487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2214,22 +2514,154 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>43884</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0.875</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="13">
+        <f>C2-B2</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>43885</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0.875</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="13">
+        <f t="shared" ref="E3:E9" si="0">C3-B3</f>
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>43886</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.6875</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="13">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>43887</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>43888</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>43889</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0.625</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="0"/>
+        <v>2.083333333333337E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>43890</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0.625</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="13">
+        <f t="shared" si="0"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="20" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="13">
         <f>SUM(E2:E19)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="21" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D21" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="13">
         <f>E20+'Week 7'!E21</f>
-        <v>1.7986111111111103</v>
+        <v>2.1111111111111103</v>
       </c>
     </row>
   </sheetData>
@@ -2237,7 +2669,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Verdana,Bold"&amp;14Internet Technologies Project Time Sheet</oddHeader>
+    <oddHeader>&amp;C&amp;"Verdana,Bold"&amp;14Internet Technologies Project Time Sheet&amp;RBen Harwood</oddHeader>
     <oddFooter>&amp;C &amp;A</oddFooter>
   </headerFooter>
   <extLst>
@@ -2294,7 +2726,7 @@
       </c>
       <c r="E21">
         <f>E20+'Week 8'!E21</f>
-        <v>1.7986111111111103</v>
+        <v>2.1111111111111103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>